<commit_message>
write results to output files
</commit_message>
<xml_diff>
--- a/results/modules_top_over_represented_go_terms_and_hub_genes.xlsx
+++ b/results/modules_top_over_represented_go_terms_and_hub_genes.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">ontology</t>
   </si>
   <si>
-    <t xml:space="preserve">hub_genes</t>
+    <t xml:space="preserve">hub_gene</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -286,6 +286,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -370,18 +371,19 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>

</xml_diff>